<commit_message>
app.iml and excel file changes
</commit_message>
<xml_diff>
--- a/Cross-Validation SVM/1 - 30obs 10features/cross-validation results.xlsx
+++ b/Cross-Validation SVM/1 - 30obs 10features/cross-validation results.xlsx
@@ -222,9 +222,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2828925" cy="3192412"/>
     <xdr:sp macro="" textlink="">
@@ -234,7 +234,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6305550" y="142874"/>
+          <a:off x="6276975" y="476249"/>
           <a:ext cx="2828925" cy="3192412"/>
         </a:xfrm>
         <a:prstGeom prst="rect">

</xml_diff>